<commit_message>
Nueva corrida generación de especificaciones.
</commit_message>
<xml_diff>
--- a/docs/datasets-especificaciones/calidad-aire-campos.xlsx
+++ b/docs/datasets-especificaciones/calidad-aire-campos.xlsx
@@ -550,7 +550,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>-401.808.541.022.993</t>
+          <t>-40.1808541022993</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -588,7 +588,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>-7.131.843.600.000.000</t>
+          <t>-71.31843</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">

</xml_diff>